<commit_message>
updated offline meter data template file
</commit_message>
<xml_diff>
--- a/myems-normalization/offline_meter_data.xlsx
+++ b/myems-normalization/offline_meter_data.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowWidth="26970" windowHeight="12450"/>
   </bookViews>
   <sheets>
-    <sheet name="能耗" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>年</t>
   </si>
@@ -28,65 +28,58 @@
     <t>日</t>
   </si>
   <si>
-    <t>用电设备</t>
-  </si>
-  <si>
-    <t>CHILLER1</t>
+    <t>offline meter</t>
   </si>
   <si>
     <r>
-      <t>离心机用电分摊（</t>
+      <t>﻿</t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
+        <sz val="9.75"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>KWH</t>
+      <t>Example Offline Meter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>﻿</t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
+        <sz val="9.75"/>
+        <rFont val="open sans"/>
         <charset val="134"/>
       </rPr>
-      <t>）</t>
+      <t>Example Offline Meter</t>
     </r>
   </si>
   <si>
-    <t>CHILLER2</t>
+    <t>如果本月缺失29/30/31日则留空</t>
   </si>
   <si>
-    <r>
-      <t>冷冻水用电分摊（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>KWH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
+    <t>确认修改A2单元格年和B2单元格月的值</t>
   </si>
   <si>
-    <t>Comp. Air</t>
+    <t>此文件仅存储一个月的数据，每个月需新建一个文件，文件名如offlinemeters-water202101.xlsx</t>
   </si>
   <si>
-    <t>压缩空气用电分摊（KWH）</t>
+    <t>此文件可以重复上传，例如每天增加前日数据后上传，系统自动读取新增的数据</t>
+  </si>
+  <si>
+    <t>如修改已经上传过的日期数据，系统可以覆盖原始数据，但需要管理员手动清除受影响的汇总数据后重启计算</t>
+  </si>
+  <si>
+    <t>“说明”列可以留空</t>
+  </si>
+  <si>
+    <t>A3,A4单元格ID不可修改</t>
+  </si>
+  <si>
+    <t>使用管理员权限账号登录管理系统，打开 '系统管理|计量表管理|离线表文件' 页面上传文件</t>
   </si>
 </sst>
 </file>
@@ -94,10 +87,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -120,6 +113,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -132,14 +131,20 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -151,8 +156,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="56"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="56"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color indexed="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="56"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -166,7 +226,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="62"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -174,57 +253,6 @@
       <i/>
       <sz val="11"/>
       <color indexed="23"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="56"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="60"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="63"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="20"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -236,50 +264,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="9.75"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="56"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="56"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
+      <sz val="9.75"/>
+      <name val="open sans"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -298,6 +290,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="36"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="46"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="29"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="30"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="62"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -305,126 +417,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="52"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="46"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="30"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="62"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="29"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="53"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="36"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="49"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,11 +445,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="30"/>
+      <left style="double">
+        <color indexed="63"/>
+      </left>
+      <right style="double">
+        <color indexed="63"/>
+      </right>
+      <top style="double">
+        <color indexed="63"/>
+      </top>
+      <bottom style="double">
+        <color indexed="63"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,17 +475,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="23"/>
-      </left>
-      <right style="thin">
-        <color indexed="23"/>
-      </right>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="23"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,17 +519,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="63"/>
+      <left style="thin">
+        <color indexed="23"/>
       </left>
-      <right style="double">
-        <color indexed="63"/>
+      <right style="thin">
+        <color indexed="23"/>
       </right>
-      <top style="double">
-        <color indexed="63"/>
+      <top style="thin">
+        <color indexed="23"/>
       </top>
-      <bottom style="double">
-        <color indexed="63"/>
+      <bottom style="thin">
+        <color indexed="23"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,8 +537,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color indexed="62"/>
+      <bottom style="medium">
+        <color indexed="30"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,169 +551,160 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -739,30 +731,26 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1190,16 +1178,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.1" customHeight="1" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.1" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="11.5037037037037" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2222222222222" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.1259259259259" style="1" customWidth="1"/>
     <col min="4" max="10" width="9" style="2"/>
     <col min="11" max="11" width="11.2518518518519" style="2" customWidth="1"/>
@@ -1313,10 +1301,10 @@
     </row>
     <row r="2" customHeight="1" spans="1:34">
       <c r="A2" s="5">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>4</v>
@@ -1422,325 +1410,192 @@
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12">
-        <v>960.899999999992</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="D3" s="11">
+        <v>999</v>
+      </c>
+      <c r="E3" s="11">
         <v>341.699999999983</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>241.500000000005</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>515.100000000002</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>124.500000000016</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>436.799999999985</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>343.200000000015</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>304.199999999983</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <v>0</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <v>167.700000000004</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <v>106.499999999978</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <v>195</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <v>183.300000000017</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <v>0</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <v>40.2999999999975</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <v>0</v>
       </c>
-      <c r="V3" s="12">
+      <c r="V3" s="11">
         <v>271.799999999985</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="11">
         <v>753.000000000011</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <v>511.199999999999</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="11">
         <v>452.100000000019</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="11">
         <v>595.199999999977</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="11">
         <v>61.7000000000098</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="11">
         <v>701.699999999983</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="11">
         <v>698.100000000013</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AD3" s="11">
         <v>419.699999999993</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>643.800000000001</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AF3" s="11">
         <v>707.700000000004</v>
       </c>
-      <c r="AG3" s="12">
+      <c r="AG3" s="11">
         <v>999.599999999991</v>
       </c>
-      <c r="AH3" s="12"/>
+      <c r="AH3" s="11">
+        <v>898.8</v>
+      </c>
     </row>
-    <row r="4" ht="23.25" customHeight="1" spans="1:34">
-      <c r="A4" s="9">
+    <row r="4" customHeight="1" spans="13:21">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+    </row>
+    <row r="5" customHeight="1" spans="13:17">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" customHeight="1" spans="12:12">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:1">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+    </row>
+    <row r="10" customHeight="1" spans="1:2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
+    </row>
+    <row r="11" customHeight="1" spans="1:2">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="E4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="F4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="G4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="H4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="I4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="J4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="K4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="L4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="M4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="N4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="O4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="P4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="Q4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="R4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="S4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="T4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="U4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="V4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="W4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="X4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="Y4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="Z4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AA4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AB4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AC4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AD4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AE4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AF4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AG4" s="12">
-        <v>4241</v>
-      </c>
-      <c r="AH4" s="12"/>
     </row>
-    <row r="5" ht="26.25" customHeight="1" spans="1:34">
-      <c r="A5" s="9">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="12" customHeight="1" spans="1:2">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
+    </row>
+    <row r="13" customHeight="1" spans="1:2">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12">
-        <v>19484</v>
-      </c>
-      <c r="E5" s="12">
-        <v>20872</v>
-      </c>
-      <c r="F5" s="12">
-        <v>30605</v>
-      </c>
-      <c r="G5" s="12">
-        <v>21887</v>
-      </c>
-      <c r="H5" s="12">
-        <v>21880</v>
-      </c>
-      <c r="I5" s="12">
-        <v>23517</v>
-      </c>
-      <c r="J5" s="12">
-        <v>31821</v>
-      </c>
-      <c r="K5" s="12">
-        <v>29922</v>
-      </c>
-      <c r="L5" s="12">
-        <v>20237</v>
-      </c>
-      <c r="M5" s="12">
-        <v>11898</v>
-      </c>
-      <c r="N5" s="12">
-        <v>17064</v>
-      </c>
-      <c r="O5" s="12">
-        <v>23744</v>
-      </c>
-      <c r="P5" s="12">
-        <v>20464</v>
-      </c>
-      <c r="Q5" s="12">
-        <v>20034</v>
-      </c>
-      <c r="R5" s="12">
-        <v>21245</v>
-      </c>
-      <c r="S5" s="12">
-        <v>24728</v>
-      </c>
-      <c r="T5" s="12">
-        <v>3098</v>
-      </c>
-      <c r="U5" s="12">
-        <v>11824</v>
-      </c>
-      <c r="V5" s="12">
-        <v>24663</v>
-      </c>
-      <c r="W5" s="12">
-        <v>28096</v>
-      </c>
-      <c r="X5" s="12">
-        <v>22219</v>
-      </c>
-      <c r="Y5" s="12">
-        <v>13918</v>
-      </c>
-      <c r="Z5" s="12">
-        <v>16849</v>
-      </c>
-      <c r="AA5" s="12">
-        <v>9520</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>8263</v>
-      </c>
-      <c r="AC5" s="12">
-        <v>19884</v>
-      </c>
-      <c r="AD5" s="12">
-        <v>24919</v>
-      </c>
-      <c r="AE5" s="12">
-        <v>30222</v>
-      </c>
-      <c r="AF5" s="12">
-        <v>21202</v>
-      </c>
-      <c r="AG5" s="12">
-        <v>19414</v>
-      </c>
-      <c r="AH5" s="12"/>
     </row>
-    <row r="6" customHeight="1" spans="13:21">
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
+    <row r="14" customHeight="1" spans="1:2">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" customHeight="1" spans="13:17">
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+    <row r="15" customHeight="1" spans="1:2">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" customHeight="1" spans="12:12">
-      <c r="L8" s="2"/>
+    <row r="16" customHeight="1" spans="1:2">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:2">
+      <c r="A17" s="1">
+        <v>8</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>

</xml_diff>